<commit_message>
add bloc4 explaination and test_dataset_real_time
</commit_message>
<xml_diff>
--- a/Referentiel_master_RNCP/documents explicatifs/brouillon/brouillon Grille toutes les infos rassembler.xlsx
+++ b/Referentiel_master_RNCP/documents explicatifs/brouillon/brouillon Grille toutes les infos rassembler.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaeta\Documents\Datapipeline_project_master\Referentiel_master_RNCP\brouillon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GaetanCORIN\Desktop\Datapipeline_comparaison_official_vs_gas_stations_reporting\Referentiel_master_RNCP\documents explicatifs\brouillon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318519F6-C04E-475D-AEED-1F339C4ED971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8918C8BC-9FE6-4D56-9395-6DA1A0C1725F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="75" windowWidth="27360" windowHeight="15180" activeTab="1" xr2:uid="{AB6F6693-6B8C-4684-9576-BC4DD09BE9E0}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{AB6F6693-6B8C-4684-9576-BC4DD09BE9E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Grille Eval Bloc1" sheetId="2" r:id="rId1"/>
@@ -567,15 +567,6 @@
     <t>Une présentation du système de supervision</t>
   </si>
   <si>
-    <t xml:space="preserve">
-La présentation du système de supervision permet d’identifier :
--	Les éléments et les indicateurs à surveiller
--	Les choix et la configuration des outils de supervision
--	La visualisation des indicateurs
--	Le système d’alertes 
-Le système de supervision permet de surveiller le bon fonctionnement de l’infrastructure.</t>
-  </si>
-  <si>
     <t>Une feuille de route d’exploitation</t>
   </si>
   <si>
@@ -900,6 +891,14 @@
   <si>
     <t xml:space="preserve">BLOC 3 : ELABORER ET PILOTER UN PROJET DATA
 20 PAGES MAX </t>
+  </si>
+  <si>
+    <t>La présentation du système de supervision permet d’identifier :
+-	Les éléments et les indicateurs à surveiller
+-	Les choix et la configuration des outils de supervision
+-	La visualisation des indicateurs
+-	Le système d’alertes 
+Le système de supervision permet de surveiller le bon fonctionnement de l’infrastructure.</t>
   </si>
 </sst>
 </file>
@@ -1606,35 +1605,35 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1979,9 +1978,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2019,7 +2018,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2125,7 +2124,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2267,7 +2266,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2284,19 +2283,19 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="70.5703125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="16.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="70.54296875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.6">
       <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
@@ -2308,9 +2307,9 @@
       <c r="G1" s="63"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="18.5" x14ac:dyDescent="0.5">
       <c r="A2" s="64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
@@ -2320,7 +2319,7 @@
       <c r="G2" s="66"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="15"/>
@@ -2329,7 +2328,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
@@ -2343,7 +2342,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="67" t="s">
         <v>4</v>
       </c>
@@ -2354,7 +2353,7 @@
       <c r="D5" s="70"/>
       <c r="E5" s="55"/>
     </row>
-    <row r="6" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -2363,7 +2362,7 @@
       <c r="F6" s="13"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:8" s="30" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="30" customFormat="1" ht="28.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
@@ -2377,7 +2376,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F7" s="27" t="s">
         <v>9</v>
@@ -2387,9 +2386,9 @@
       </c>
       <c r="H7" s="29"/>
     </row>
-    <row r="8" spans="1:8" s="5" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="5" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="58" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B8" s="57" t="s">
         <v>25</v>
@@ -2401,13 +2400,13 @@
         <v>27</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="19"/>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="5" customFormat="1" ht="118.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="59"/>
       <c r="B9" s="17" t="s">
         <v>28</v>
@@ -2419,13 +2418,13 @@
         <v>30</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="19"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" ht="99.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="5" customFormat="1" ht="99.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="59"/>
       <c r="B10" s="17" t="s">
         <v>31</v>
@@ -2437,13 +2436,13 @@
         <v>33</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="19"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" ht="75.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="5" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="59"/>
       <c r="B11" s="17" t="s">
         <v>34</v>
@@ -2455,13 +2454,13 @@
         <v>36</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="5" customFormat="1" ht="68.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="59"/>
       <c r="B12" s="56" t="s">
         <v>37</v>
@@ -2473,13 +2472,13 @@
         <v>39</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="19"/>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="5" customFormat="1" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="59"/>
       <c r="B13" s="17" t="s">
         <v>40</v>
@@ -2491,13 +2490,13 @@
         <v>42</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="19"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="5" customFormat="1" ht="112" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="59"/>
       <c r="B14" s="56" t="s">
         <v>43</v>
@@ -2509,13 +2508,13 @@
         <v>45</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="19"/>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="5" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="59"/>
       <c r="B15" s="56" t="s">
         <v>46</v>
@@ -2527,13 +2526,13 @@
         <v>48</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="19"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="70" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="59"/>
       <c r="B16" s="45" t="s">
         <v>49</v>
@@ -2545,13 +2544,13 @@
         <v>51</v>
       </c>
       <c r="E16" s="45" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F16" s="44"/>
       <c r="G16" s="46"/>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:8" ht="90.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="90.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="60"/>
       <c r="B17" s="21" t="s">
         <v>52</v>
@@ -2563,13 +2562,13 @@
         <v>54</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="23"/>
       <c r="H17" s="10"/>
     </row>
-    <row r="18" spans="1:8" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A18" s="31"/>
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
@@ -2580,12 +2579,12 @@
       </c>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B19" s="33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="3" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
@@ -2598,7 +2597,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="3" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
         <v>14</v>
       </c>
@@ -2611,7 +2610,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B22" s="34" t="s">
         <v>15</v>
       </c>
@@ -2651,23 +2650,23 @@
   </sheetPr>
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="70.5703125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="15.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="70.54296875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.6">
       <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
@@ -2679,9 +2678,9 @@
       <c r="G1" s="63"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="18.5" x14ac:dyDescent="0.5">
       <c r="A2" s="64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
@@ -2691,7 +2690,7 @@
       <c r="G2" s="66"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="15"/>
@@ -2700,7 +2699,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
@@ -2714,7 +2713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="67" t="s">
         <v>4</v>
       </c>
@@ -2725,7 +2724,7 @@
       <c r="D5" s="70"/>
       <c r="E5" s="55"/>
     </row>
-    <row r="6" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -2734,7 +2733,7 @@
       <c r="F6" s="13"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:8" s="30" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="30" customFormat="1" ht="28.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
@@ -2748,7 +2747,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F7" s="27" t="s">
         <v>9</v>
@@ -2758,9 +2757,9 @@
       </c>
       <c r="H7" s="29"/>
     </row>
-    <row r="8" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="5" customFormat="1" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A8" s="58" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>56</v>
@@ -2772,13 +2771,13 @@
         <v>58</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="19"/>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="5" customFormat="1" ht="46" x14ac:dyDescent="0.35">
       <c r="A9" s="59"/>
       <c r="B9" s="56" t="s">
         <v>59</v>
@@ -2790,13 +2789,13 @@
         <v>61</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="19"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="5" customFormat="1" ht="46" x14ac:dyDescent="0.35">
       <c r="A10" s="59"/>
       <c r="B10" s="56" t="s">
         <v>62</v>
@@ -2808,13 +2807,13 @@
         <v>64</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="19"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="5" customFormat="1" ht="69" x14ac:dyDescent="0.35">
       <c r="A11" s="59"/>
       <c r="B11" s="17" t="s">
         <v>65</v>
@@ -2826,13 +2825,13 @@
         <v>67</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="5" customFormat="1" ht="92" x14ac:dyDescent="0.35">
       <c r="A12" s="59"/>
       <c r="B12" s="56" t="s">
         <v>68</v>
@@ -2844,13 +2843,13 @@
         <v>70</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="19"/>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="5" customFormat="1" ht="46" x14ac:dyDescent="0.35">
       <c r="A13" s="59"/>
       <c r="B13" s="17" t="s">
         <v>71</v>
@@ -2862,13 +2861,13 @@
         <v>73</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="19"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="59"/>
       <c r="B14" s="17" t="s">
         <v>74</v>
@@ -2880,13 +2879,13 @@
         <v>76</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="19"/>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:8" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="60"/>
       <c r="B15" s="21" t="s">
         <v>77</v>
@@ -2898,13 +2897,13 @@
         <v>79</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F15" s="51"/>
       <c r="G15" s="23"/>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:8" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A16" s="31"/>
       <c r="B16" s="14"/>
       <c r="C16" s="15"/>
@@ -2915,12 +2914,12 @@
       </c>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B17" s="33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" s="3" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
         <v>13</v>
       </c>
@@ -2933,7 +2932,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" s="3" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>14</v>
       </c>
@@ -2946,7 +2945,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B20" s="34" t="s">
         <v>15</v>
       </c>
@@ -2990,19 +2989,19 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="70.5703125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="14.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="70.54296875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.6">
       <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
@@ -3014,9 +3013,9 @@
       <c r="G1" s="63"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="18.5" x14ac:dyDescent="0.5">
       <c r="A2" s="64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
@@ -3026,7 +3025,7 @@
       <c r="G2" s="66"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="15"/>
@@ -3035,7 +3034,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
@@ -3049,7 +3048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="67" t="s">
         <v>4</v>
       </c>
@@ -3060,7 +3059,7 @@
       <c r="D5" s="70"/>
       <c r="E5" s="55"/>
     </row>
-    <row r="6" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -3069,7 +3068,7 @@
       <c r="F6" s="13"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:8" s="30" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="30" customFormat="1" ht="28.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
@@ -3083,7 +3082,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F7" s="27" t="s">
         <v>9</v>
@@ -3093,9 +3092,9 @@
       </c>
       <c r="H7" s="29"/>
     </row>
-    <row r="8" spans="1:8" s="5" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="5" customFormat="1" ht="69" x14ac:dyDescent="0.35">
       <c r="A8" s="58" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>81</v>
@@ -3111,7 +3110,7 @@
       <c r="G8" s="19"/>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="5" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="59"/>
       <c r="B9" s="56" t="s">
         <v>84</v>
@@ -3127,7 +3126,7 @@
       <c r="G9" s="19"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="5" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="59"/>
       <c r="B10" s="17" t="s">
         <v>87</v>
@@ -3143,7 +3142,7 @@
       <c r="G10" s="19"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" ht="108" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="5" customFormat="1" ht="149.5" x14ac:dyDescent="0.35">
       <c r="A11" s="59"/>
       <c r="B11" s="56" t="s">
         <v>90</v>
@@ -3155,13 +3154,13 @@
         <v>92</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="5" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="59"/>
       <c r="B12" s="56" t="s">
         <v>93</v>
@@ -3173,13 +3172,13 @@
         <v>95</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="19"/>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="5" customFormat="1" ht="115.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="59"/>
       <c r="B13" s="17" t="s">
         <v>96</v>
@@ -3195,7 +3194,7 @@
       <c r="G13" s="19"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="5" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="59"/>
       <c r="B14" s="17" t="s">
         <v>99</v>
@@ -3211,7 +3210,7 @@
       <c r="G14" s="19"/>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="5" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="59"/>
       <c r="B15" s="17" t="s">
         <v>102</v>
@@ -3223,13 +3222,13 @@
         <v>104</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="19"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="59"/>
       <c r="B16" s="45" t="s">
         <v>105</v>
@@ -3245,7 +3244,7 @@
       <c r="G16" s="46"/>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:8" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="60"/>
       <c r="B17" s="21" t="s">
         <v>108</v>
@@ -3261,7 +3260,7 @@
       <c r="G17" s="23"/>
       <c r="H17" s="10"/>
     </row>
-    <row r="18" spans="1:8" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A18" s="31"/>
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
@@ -3272,12 +3271,12 @@
       </c>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B19" s="33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="3" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
@@ -3290,7 +3289,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="3" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
         <v>14</v>
       </c>
@@ -3303,7 +3302,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B22" s="34" t="s">
         <v>15</v>
       </c>
@@ -3344,22 +3343,22 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="62.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="70.5703125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="14.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="62.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="70.54296875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.6">
       <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
@@ -3370,9 +3369,9 @@
       <c r="F1" s="63"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.5" x14ac:dyDescent="0.5">
       <c r="A2" s="64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
@@ -3381,7 +3380,7 @@
       <c r="F2" s="66"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="15"/>
@@ -3389,7 +3388,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
@@ -3402,7 +3401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="67" t="s">
         <v>4</v>
       </c>
@@ -3412,7 +3411,7 @@
       </c>
       <c r="D5" s="70"/>
     </row>
-    <row r="6" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -3420,7 +3419,7 @@
       <c r="E6" s="13"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="30" customFormat="1" ht="28.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
@@ -3441,9 +3440,9 @@
       </c>
       <c r="G7" s="29"/>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="71" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>112</v>
@@ -3458,7 +3457,7 @@
       <c r="F8" s="19"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="115" x14ac:dyDescent="0.35">
       <c r="A9" s="59"/>
       <c r="B9" s="17" t="s">
         <v>119</v>
@@ -3473,7 +3472,7 @@
       <c r="F9" s="19"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="5" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="59"/>
       <c r="B10" s="56" t="s">
         <v>122</v>
@@ -3488,7 +3487,7 @@
       <c r="F10" s="19"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" s="5" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="5" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="59"/>
       <c r="B11" s="56" t="s">
         <v>125</v>
@@ -3503,7 +3502,7 @@
       <c r="F11" s="19"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="59"/>
       <c r="B12" s="56" t="s">
         <v>128</v>
@@ -3518,7 +3517,7 @@
       <c r="F12" s="19"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" s="5" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="5" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="59"/>
       <c r="B13" s="17" t="s">
         <v>113</v>
@@ -3527,73 +3526,73 @@
         <v>131</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>132</v>
+        <v>205</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="19"/>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="5" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="59"/>
       <c r="B14" s="17" t="s">
         <v>114</v>
       </c>
       <c r="C14" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" s="35" t="s">
         <v>133</v>
-      </c>
-      <c r="D14" s="35" t="s">
-        <v>134</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="19"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="5" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="59"/>
       <c r="B15" s="17" t="s">
         <v>115</v>
       </c>
       <c r="C15" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" s="35" t="s">
         <v>135</v>
-      </c>
-      <c r="D15" s="35" t="s">
-        <v>136</v>
       </c>
       <c r="E15" s="18"/>
       <c r="F15" s="19"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="59"/>
       <c r="B16" s="17" t="s">
         <v>116</v>
       </c>
       <c r="C16" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>138</v>
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="20"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="60"/>
       <c r="B17" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="D17" s="21" t="s">
         <v>140</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>141</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="23"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A18" s="31"/>
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
@@ -3603,12 +3602,12 @@
       </c>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B19" s="33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="3" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
@@ -3621,7 +3620,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="3" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
         <v>14</v>
       </c>
@@ -3634,7 +3633,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B22" s="34" t="s">
         <v>15</v>
       </c>
@@ -3679,18 +3678,18 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="70.5703125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="19.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="70.54296875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.6">
       <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
@@ -3701,9 +3700,9 @@
       <c r="F1" s="63"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.5" x14ac:dyDescent="0.5">
       <c r="A2" s="64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
@@ -3712,7 +3711,7 @@
       <c r="F2" s="66"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="15"/>
@@ -3720,7 +3719,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
@@ -3733,7 +3732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="67" t="s">
         <v>4</v>
       </c>
@@ -3743,7 +3742,7 @@
       </c>
       <c r="D5" s="70"/>
     </row>
-    <row r="6" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -3751,7 +3750,7 @@
       <c r="E6" s="13"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="30" customFormat="1" ht="28.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
@@ -3772,174 +3771,174 @@
       </c>
       <c r="G7" s="29"/>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A8" s="71" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>57</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="19"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="69" x14ac:dyDescent="0.35">
       <c r="A9" s="59"/>
       <c r="B9" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="D9" s="17" t="s">
         <v>146</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>147</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="19"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="5" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="59"/>
       <c r="B10" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="D10" s="17" t="s">
         <v>149</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>150</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="19"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" s="5" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="5" customFormat="1" ht="45.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="59"/>
       <c r="B11" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="D11" s="35" t="s">
         <v>152</v>
-      </c>
-      <c r="D11" s="35" t="s">
-        <v>153</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="19"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="46" x14ac:dyDescent="0.35">
       <c r="A12" s="59"/>
       <c r="B12" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="D12" s="35" t="s">
         <v>155</v>
-      </c>
-      <c r="D12" s="35" t="s">
-        <v>156</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="19"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" s="5" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="5" customFormat="1" ht="69" x14ac:dyDescent="0.35">
       <c r="A13" s="59"/>
       <c r="B13" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="D13" s="35" t="s">
         <v>158</v>
-      </c>
-      <c r="D13" s="35" t="s">
-        <v>159</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="19"/>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="5" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="59"/>
       <c r="B14" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="D14" s="35" t="s">
         <v>161</v>
-      </c>
-      <c r="D14" s="35" t="s">
-        <v>162</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="19"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="5" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="59"/>
       <c r="B15" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C15" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="D15" s="35" t="s">
         <v>163</v>
-      </c>
-      <c r="D15" s="35" t="s">
-        <v>164</v>
       </c>
       <c r="E15" s="18"/>
       <c r="F15" s="19"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" s="5" customFormat="1" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="5" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="59"/>
       <c r="B16" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C16" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="D16" s="35" t="s">
         <v>166</v>
-      </c>
-      <c r="D16" s="35" t="s">
-        <v>167</v>
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="19"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="1:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="59"/>
       <c r="B17" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="D17" s="17" t="s">
         <v>169</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>170</v>
       </c>
       <c r="E17" s="18"/>
       <c r="F17" s="20"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" ht="84.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="60"/>
       <c r="B18" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="D18" s="21" t="s">
         <v>172</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>173</v>
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="23"/>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A19" s="31"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -3949,12 +3948,12 @@
       </c>
       <c r="F19" s="14"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B20" s="33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="3" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
         <v>13</v>
       </c>
@@ -3967,7 +3966,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="3" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
@@ -3980,7 +3979,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B23" s="34" t="s">
         <v>15</v>
       </c>
@@ -4024,18 +4023,18 @@
       <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="65" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="39" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="20.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="70.5703125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.85546875" style="1"/>
+    <col min="3" max="3" width="11.81640625" style="39" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="20.54296875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="70.54296875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.6">
       <c r="A1" s="61" t="s">
         <v>18</v>
       </c>
@@ -4047,9 +4046,9 @@
       <c r="G1" s="63"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="18.5" x14ac:dyDescent="0.5">
       <c r="A2" s="64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
@@ -4059,7 +4058,7 @@
       <c r="G2" s="66"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="6"/>
@@ -4068,7 +4067,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
@@ -4076,13 +4075,13 @@
       <c r="C4" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="79"/>
+      <c r="D4" s="74"/>
       <c r="E4" s="70"/>
       <c r="G4" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="67" t="s">
         <v>4</v>
       </c>
@@ -4090,10 +4089,10 @@
       <c r="C5" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="79"/>
+      <c r="D5" s="74"/>
       <c r="E5" s="70"/>
     </row>
-    <row r="6" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="4"/>
@@ -4102,7 +4101,7 @@
       <c r="F6" s="13"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:8" s="30" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="30" customFormat="1" ht="14.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
@@ -4126,7 +4125,7 @@
       </c>
       <c r="H7" s="29"/>
     </row>
-    <row r="8" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A8" s="58" t="s">
         <v>24</v>
       </c>
@@ -4134,141 +4133,141 @@
         <v>25</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D8" s="38"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="80"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="76"/>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A9" s="59"/>
       <c r="B9" s="17" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D9" s="38"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="77"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="73"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="5" customFormat="1" ht="23" x14ac:dyDescent="0.35">
       <c r="A10" s="59"/>
       <c r="B10" s="17" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D10" s="38"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="77"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="73"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A11" s="59"/>
       <c r="B11" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D11" s="38"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="77"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="73"/>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="5" customFormat="1" ht="46" x14ac:dyDescent="0.35">
       <c r="A12" s="59"/>
       <c r="B12" s="17" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D12" s="38"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="77"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="73"/>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A13" s="59"/>
       <c r="B13" s="17" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D13" s="38"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="77"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="73"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="5" customFormat="1" ht="23" x14ac:dyDescent="0.35">
       <c r="A14" s="59"/>
       <c r="B14" s="17" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D14" s="38"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="77"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="73"/>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A15" s="59"/>
       <c r="B15" s="17" t="s">
         <v>46</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D15" s="38"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="77"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="73"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="5" customFormat="1" ht="46" x14ac:dyDescent="0.35">
       <c r="A16" s="59"/>
       <c r="B16" s="17" t="s">
         <v>49</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D16" s="38"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="77"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="73"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="5" customFormat="1" ht="58" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="60"/>
       <c r="B17" s="45" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D17" s="36"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="77"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="73"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="5" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A18" s="75" t="s">
         <v>55</v>
       </c>
@@ -4276,113 +4275,113 @@
         <v>56</v>
       </c>
       <c r="C18" s="43" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D18" s="43"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="76"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="72"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A19" s="59"/>
       <c r="B19" s="17" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D19" s="47"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="77"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="73"/>
       <c r="H19" s="9"/>
     </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="5" customFormat="1" ht="23" x14ac:dyDescent="0.35">
       <c r="A20" s="59"/>
       <c r="B20" s="17" t="s">
         <v>62</v>
       </c>
       <c r="C20" s="50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D20" s="47"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="77"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="73"/>
       <c r="H20" s="9"/>
     </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A21" s="59"/>
       <c r="B21" s="17" t="s">
         <v>65</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D21" s="47"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="77"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="73"/>
       <c r="H21" s="9"/>
     </row>
-    <row r="22" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="5" customFormat="1" ht="46" x14ac:dyDescent="0.35">
       <c r="A22" s="59"/>
       <c r="B22" s="17" t="s">
         <v>68</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D22" s="47"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="77"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="73"/>
       <c r="H22" s="9"/>
     </row>
-    <row r="23" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A23" s="59"/>
       <c r="B23" s="17" t="s">
         <v>71</v>
       </c>
       <c r="C23" s="47" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D23" s="47"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="77"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="73"/>
       <c r="H23" s="9"/>
     </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A24" s="59"/>
       <c r="B24" s="17" t="s">
         <v>74</v>
       </c>
       <c r="C24" s="47" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D24" s="47"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="77"/>
+      <c r="E24" s="78"/>
+      <c r="F24" s="78"/>
+      <c r="G24" s="73"/>
       <c r="H24" s="9"/>
     </row>
-    <row r="25" spans="1:8" s="5" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" s="5" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="60"/>
       <c r="B25" s="21" t="s">
         <v>77</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D25" s="36"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="77"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="73"/>
       <c r="H25" s="9"/>
     </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="5" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A26" s="75" t="s">
         <v>80</v>
       </c>
@@ -4390,141 +4389,141 @@
         <v>81</v>
       </c>
       <c r="C26" s="43" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D26" s="43"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="76"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="72"/>
       <c r="H26" s="9"/>
     </row>
-    <row r="27" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A27" s="59"/>
       <c r="B27" s="53" t="s">
         <v>84</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D27" s="38"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="77"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="73"/>
       <c r="H27" s="9"/>
     </row>
-    <row r="28" spans="1:8" s="5" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" s="5" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="59"/>
       <c r="B28" s="53" t="s">
         <v>87</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D28" s="38"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="77"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="73"/>
       <c r="H28" s="9"/>
     </row>
-    <row r="29" spans="1:8" s="5" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" s="5" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="59"/>
       <c r="B29" s="53" t="s">
         <v>90</v>
       </c>
       <c r="C29" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D29" s="38"/>
-      <c r="E29" s="73"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="77"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="73"/>
       <c r="H29" s="9"/>
     </row>
-    <row r="30" spans="1:8" s="5" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" s="5" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="59"/>
       <c r="B30" s="53" t="s">
         <v>93</v>
       </c>
       <c r="C30" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D30" s="38"/>
-      <c r="E30" s="73"/>
-      <c r="F30" s="73"/>
-      <c r="G30" s="77"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="73"/>
       <c r="H30" s="9"/>
     </row>
-    <row r="31" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="5" customFormat="1" ht="46" x14ac:dyDescent="0.35">
       <c r="A31" s="59"/>
       <c r="B31" s="53" t="s">
         <v>96</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D31" s="38"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="77"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="78"/>
+      <c r="G31" s="73"/>
       <c r="H31" s="9"/>
     </row>
-    <row r="32" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" s="5" customFormat="1" ht="46" x14ac:dyDescent="0.35">
       <c r="A32" s="59"/>
       <c r="B32" s="53" t="s">
         <v>99</v>
       </c>
       <c r="C32" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D32" s="38"/>
-      <c r="E32" s="73"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="77"/>
+      <c r="E32" s="78"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="73"/>
       <c r="H32" s="9"/>
     </row>
-    <row r="33" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" s="5" customFormat="1" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A33" s="59"/>
       <c r="B33" s="53" t="s">
         <v>102</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D33" s="38"/>
-      <c r="E33" s="73"/>
-      <c r="F33" s="73"/>
-      <c r="G33" s="77"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="73"/>
       <c r="H33" s="9"/>
     </row>
-    <row r="34" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A34" s="59"/>
       <c r="B34" s="53" t="s">
         <v>105</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D34" s="38"/>
-      <c r="E34" s="73"/>
-      <c r="F34" s="73"/>
-      <c r="G34" s="77"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="78"/>
+      <c r="G34" s="73"/>
       <c r="H34" s="9"/>
     </row>
-    <row r="35" spans="1:8" s="5" customFormat="1" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" s="5" customFormat="1" ht="46.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="60"/>
       <c r="B35" s="54" t="s">
         <v>108</v>
       </c>
       <c r="C35" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D35" s="36"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="73"/>
-      <c r="G35" s="77"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="78"/>
+      <c r="G35" s="73"/>
       <c r="H35" s="9"/>
     </row>
-    <row r="36" spans="1:8" s="5" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" s="5" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A36" s="75" t="s">
         <v>111</v>
       </c>
@@ -4532,297 +4531,297 @@
         <v>112</v>
       </c>
       <c r="C36" s="43" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D36" s="43"/>
-      <c r="E36" s="72"/>
-      <c r="F36" s="72"/>
-      <c r="G36" s="76"/>
+      <c r="E36" s="79"/>
+      <c r="F36" s="79"/>
+      <c r="G36" s="72"/>
       <c r="H36" s="9"/>
     </row>
-    <row r="37" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A37" s="59"/>
       <c r="B37" s="17" t="s">
         <v>119</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D37" s="38"/>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
-      <c r="G37" s="77"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="78"/>
+      <c r="G37" s="73"/>
       <c r="H37" s="9"/>
     </row>
-    <row r="38" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A38" s="59"/>
       <c r="B38" s="17" t="s">
         <v>122</v>
       </c>
       <c r="C38" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D38" s="38"/>
-      <c r="E38" s="73"/>
-      <c r="F38" s="73"/>
-      <c r="G38" s="77"/>
+      <c r="E38" s="78"/>
+      <c r="F38" s="78"/>
+      <c r="G38" s="73"/>
       <c r="H38" s="9"/>
     </row>
-    <row r="39" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A39" s="59"/>
       <c r="B39" s="17" t="s">
         <v>125</v>
       </c>
       <c r="C39" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D39" s="38"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="73"/>
-      <c r="G39" s="77"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="73"/>
       <c r="H39" s="9"/>
     </row>
-    <row r="40" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A40" s="59"/>
       <c r="B40" s="17" t="s">
         <v>128</v>
       </c>
       <c r="C40" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D40" s="38"/>
-      <c r="E40" s="73"/>
-      <c r="F40" s="73"/>
-      <c r="G40" s="77"/>
+      <c r="E40" s="78"/>
+      <c r="F40" s="78"/>
+      <c r="G40" s="73"/>
       <c r="H40" s="9"/>
     </row>
-    <row r="41" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A41" s="59"/>
       <c r="B41" s="17" t="s">
         <v>113</v>
       </c>
       <c r="C41" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D41" s="38"/>
-      <c r="E41" s="73"/>
-      <c r="F41" s="73"/>
-      <c r="G41" s="77"/>
+      <c r="E41" s="78"/>
+      <c r="F41" s="78"/>
+      <c r="G41" s="73"/>
       <c r="H41" s="9"/>
     </row>
-    <row r="42" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A42" s="59"/>
       <c r="B42" s="17" t="s">
         <v>114</v>
       </c>
       <c r="C42" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D42" s="38"/>
-      <c r="E42" s="73"/>
-      <c r="F42" s="73"/>
-      <c r="G42" s="77"/>
+      <c r="E42" s="78"/>
+      <c r="F42" s="78"/>
+      <c r="G42" s="73"/>
       <c r="H42" s="9"/>
     </row>
-    <row r="43" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A43" s="59"/>
       <c r="B43" s="17" t="s">
         <v>115</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D43" s="38"/>
-      <c r="E43" s="73"/>
-      <c r="F43" s="73"/>
-      <c r="G43" s="77"/>
+      <c r="E43" s="78"/>
+      <c r="F43" s="78"/>
+      <c r="G43" s="73"/>
       <c r="H43" s="9"/>
     </row>
-    <row r="44" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" s="5" customFormat="1" ht="23" x14ac:dyDescent="0.35">
       <c r="A44" s="59"/>
       <c r="B44" s="17" t="s">
         <v>116</v>
       </c>
       <c r="C44" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D44" s="38"/>
-      <c r="E44" s="73"/>
-      <c r="F44" s="73"/>
-      <c r="G44" s="77"/>
+      <c r="E44" s="78"/>
+      <c r="F44" s="78"/>
+      <c r="G44" s="73"/>
       <c r="H44" s="9"/>
     </row>
-    <row r="45" spans="1:8" s="5" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" s="5" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="60"/>
       <c r="B45" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C45" s="48" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D45" s="48"/>
-      <c r="E45" s="73"/>
-      <c r="F45" s="73"/>
-      <c r="G45" s="77"/>
+      <c r="E45" s="78"/>
+      <c r="F45" s="78"/>
+      <c r="G45" s="73"/>
       <c r="H45" s="9"/>
     </row>
-    <row r="46" spans="1:8" s="5" customFormat="1" ht="18.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" s="5" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A46" s="75" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="B46" s="42" t="s">
-        <v>143</v>
-      </c>
       <c r="C46" s="43" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D46" s="43"/>
-      <c r="E46" s="72"/>
-      <c r="F46" s="72"/>
-      <c r="G46" s="76"/>
+      <c r="E46" s="79"/>
+      <c r="F46" s="79"/>
+      <c r="G46" s="72"/>
       <c r="H46" s="9"/>
     </row>
-    <row r="47" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A47" s="59"/>
       <c r="B47" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C47" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D47" s="38"/>
-      <c r="E47" s="73"/>
-      <c r="F47" s="73"/>
-      <c r="G47" s="77"/>
+      <c r="E47" s="78"/>
+      <c r="F47" s="78"/>
+      <c r="G47" s="73"/>
       <c r="H47" s="9"/>
     </row>
-    <row r="48" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A48" s="59"/>
       <c r="B48" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C48" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D48" s="38"/>
-      <c r="E48" s="73"/>
-      <c r="F48" s="73"/>
-      <c r="G48" s="77"/>
+      <c r="E48" s="78"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="73"/>
       <c r="H48" s="9"/>
     </row>
-    <row r="49" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A49" s="59"/>
       <c r="B49" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C49" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D49" s="38"/>
-      <c r="E49" s="73"/>
-      <c r="F49" s="73"/>
-      <c r="G49" s="77"/>
+      <c r="E49" s="78"/>
+      <c r="F49" s="78"/>
+      <c r="G49" s="73"/>
       <c r="H49" s="9"/>
     </row>
-    <row r="50" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A50" s="59"/>
       <c r="B50" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C50" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D50" s="38"/>
-      <c r="E50" s="73"/>
-      <c r="F50" s="73"/>
-      <c r="G50" s="77"/>
+      <c r="E50" s="78"/>
+      <c r="F50" s="78"/>
+      <c r="G50" s="73"/>
       <c r="H50" s="9"/>
     </row>
-    <row r="51" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A51" s="59"/>
       <c r="B51" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C51" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D51" s="38"/>
-      <c r="E51" s="73"/>
-      <c r="F51" s="73"/>
-      <c r="G51" s="77"/>
+      <c r="E51" s="78"/>
+      <c r="F51" s="78"/>
+      <c r="G51" s="73"/>
       <c r="H51" s="9"/>
     </row>
-    <row r="52" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A52" s="59"/>
       <c r="B52" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C52" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D52" s="38"/>
-      <c r="E52" s="73"/>
-      <c r="F52" s="73"/>
-      <c r="G52" s="77"/>
+      <c r="E52" s="78"/>
+      <c r="F52" s="78"/>
+      <c r="G52" s="73"/>
       <c r="H52" s="9"/>
     </row>
-    <row r="53" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A53" s="59"/>
       <c r="B53" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C53" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D53" s="38"/>
-      <c r="E53" s="73"/>
-      <c r="F53" s="73"/>
-      <c r="G53" s="77"/>
+      <c r="E53" s="78"/>
+      <c r="F53" s="78"/>
+      <c r="G53" s="73"/>
       <c r="H53" s="9"/>
     </row>
-    <row r="54" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" s="5" customFormat="1" ht="23" x14ac:dyDescent="0.35">
       <c r="A54" s="59"/>
       <c r="B54" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C54" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D54" s="38"/>
-      <c r="E54" s="73"/>
-      <c r="F54" s="73"/>
-      <c r="G54" s="77"/>
+      <c r="E54" s="78"/>
+      <c r="F54" s="78"/>
+      <c r="G54" s="73"/>
       <c r="H54" s="9"/>
     </row>
-    <row r="55" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" s="5" customFormat="1" ht="23" x14ac:dyDescent="0.35">
       <c r="A55" s="59"/>
       <c r="B55" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C55" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D55" s="38"/>
-      <c r="E55" s="73"/>
-      <c r="F55" s="73"/>
-      <c r="G55" s="77"/>
+      <c r="E55" s="78"/>
+      <c r="F55" s="78"/>
+      <c r="G55" s="73"/>
       <c r="H55" s="9"/>
     </row>
-    <row r="56" spans="1:8" s="5" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" s="5" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="60"/>
       <c r="B56" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C56" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D56" s="36"/>
-      <c r="E56" s="74"/>
-      <c r="F56" s="74"/>
-      <c r="G56" s="78"/>
+      <c r="E56" s="80"/>
+      <c r="F56" s="80"/>
+      <c r="G56" s="81"/>
       <c r="H56" s="9"/>
     </row>
-    <row r="57" spans="1:8" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="14.5" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A57" s="14"/>
       <c r="B57" s="14"/>
       <c r="C57" s="6"/>
@@ -4831,7 +4830,7 @@
       <c r="F57" s="16"/>
       <c r="G57" s="14"/>
     </row>
-    <row r="58" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="18.5" x14ac:dyDescent="0.4">
       <c r="E58" s="40" t="s">
         <v>23</v>
       </c>
@@ -4839,6 +4838,17 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="F46:F56"/>
+    <mergeCell ref="E46:E56"/>
+    <mergeCell ref="A26:A35"/>
+    <mergeCell ref="A46:A56"/>
+    <mergeCell ref="G46:G56"/>
+    <mergeCell ref="F26:F35"/>
+    <mergeCell ref="E26:E35"/>
+    <mergeCell ref="A36:A45"/>
+    <mergeCell ref="E36:E45"/>
+    <mergeCell ref="F36:F45"/>
+    <mergeCell ref="G36:G45"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A4:B4"/>
@@ -4854,17 +4864,6 @@
     <mergeCell ref="E8:E17"/>
     <mergeCell ref="F18:F25"/>
     <mergeCell ref="E18:E25"/>
-    <mergeCell ref="F46:F56"/>
-    <mergeCell ref="E46:E56"/>
-    <mergeCell ref="A26:A35"/>
-    <mergeCell ref="A46:A56"/>
-    <mergeCell ref="G46:G56"/>
-    <mergeCell ref="F26:F35"/>
-    <mergeCell ref="E26:E35"/>
-    <mergeCell ref="A36:A45"/>
-    <mergeCell ref="E36:E45"/>
-    <mergeCell ref="F36:F45"/>
-    <mergeCell ref="G36:G45"/>
   </mergeCells>
   <conditionalFormatting sqref="F58">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
@@ -4896,26 +4895,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="1ba08013-ef1c-4130-a497-bc53eb55e168" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ed22885-9a1c-4a78-8ce9-dd4492997226">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010097798227B93F3B46A4C8EE6693783472" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="07a0dc2af2640077c1870da1684932dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1ba08013-ef1c-4130-a497-bc53eb55e168" xmlns:ns3="0ed22885-9a1c-4a78-8ce9-dd4492997226" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9f8b351a6a60032acdf3e22257ff17f6" ns2:_="" ns3:_="">
     <xsd:import namespace="1ba08013-ef1c-4130-a497-bc53eb55e168"/>
@@ -5144,28 +5123,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6771D95-FB55-4106-9918-F95569952A80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="81d943eb-53de-4d5a-93c5-961cb00f222e"/>
-    <ds:schemaRef ds:uri="11399b42-56c9-44ff-9016-8ae70501af32"/>
-    <ds:schemaRef ds:uri="1ba08013-ef1c-4130-a497-bc53eb55e168"/>
-    <ds:schemaRef ds:uri="0ed22885-9a1c-4a78-8ce9-dd4492997226"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{801D0CEA-46D1-40C8-94B1-8478A557036E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="1ba08013-ef1c-4130-a497-bc53eb55e168" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ed22885-9a1c-4a78-8ce9-dd4492997226">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B35CE1C-889F-46C7-9B5C-5C98D0751230}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5182,4 +5160,25 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{801D0CEA-46D1-40C8-94B1-8478A557036E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6771D95-FB55-4106-9918-F95569952A80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="81d943eb-53de-4d5a-93c5-961cb00f222e"/>
+    <ds:schemaRef ds:uri="11399b42-56c9-44ff-9016-8ae70501af32"/>
+    <ds:schemaRef ds:uri="1ba08013-ef1c-4130-a497-bc53eb55e168"/>
+    <ds:schemaRef ds:uri="0ed22885-9a1c-4a78-8ce9-dd4492997226"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>